<commit_message>
feat: Log DRLs from DecisionTable, update data type name of update-auto-assignment dto, add auto-assignment-rule dto,  update insertRuleTableData, add getRuleTableData in excel-manipulation service, add getAutoAssignmentSettings in auto-assignment service, add getAutoAssignmentSettings in auto-assignment controller
</commit_message>
<xml_diff>
--- a/droolsServer/src/main/resources/dtables/drools_decisiontable.drl.xlsx
+++ b/droolsServer/src/main/resources/dtables/drools_decisiontable.drl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Smashminton\droolsServer\src\main\resources\dtables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Ex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE72D8A9-CDDD-4E50-A716-1E8335A45F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7574F11B-262B-48D1-B242-6948CE1B7BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BFDAF6E-2941-4913-A8C6-9531DFE6061F}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="113">
-  <si>
-    <t>Max Shifts Per Day</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="114">
   <si>
     <t>RuleSet</t>
   </si>
@@ -59,15 +56,6 @@
     <t>CONDITION</t>
   </si>
   <si>
-    <t>Max Shift Per Week</t>
-  </si>
-  <si>
-    <t>isEligible?</t>
-  </si>
-  <si>
-    <t>Max Employees Per Shift</t>
-  </si>
-  <si>
     <t>Nhân viên có thể phân công</t>
   </si>
   <si>
@@ -128,21 +116,12 @@
     <t>-</t>
   </si>
   <si>
-    <t>isAssignable?</t>
-  </si>
-  <si>
     <t>eligible == $1</t>
   </si>
   <si>
     <t>assignable == $1</t>
   </si>
   <si>
-    <t>setEligible</t>
-  </si>
-  <si>
-    <t>setAssignable</t>
-  </si>
-  <si>
     <t>getSize() &gt; $1</t>
   </si>
   <si>
@@ -167,9 +146,6 @@
     <t>EmployeeRule</t>
   </si>
   <si>
-    <t>isAlreadyAssigned?</t>
-  </si>
-  <si>
     <t>System.out.println($1);</t>
   </si>
   <si>
@@ -242,12 +218,6 @@
     <t>"Set Assigble For: " + $SD</t>
   </si>
   <si>
-    <t>AutoAssignmentContext</t>
-  </si>
-  <si>
-    <t>CurrentShift</t>
-  </si>
-  <si>
     <t>"Set Eligible For: " + $E + " on " + $CSD</t>
   </si>
   <si>
@@ -299,9 +269,6 @@
     <t>SecondRuleEnrollmentShift</t>
   </si>
   <si>
-    <t>isEnrolled?</t>
-  </si>
-  <si>
     <t>ShiftEnrollment(getShift().equals($SD))</t>
   </si>
   <si>
@@ -311,9 +278,6 @@
     <t>setDeletable(true);</t>
   </si>
   <si>
-    <t>setDeletable</t>
-  </si>
-  <si>
     <t>FirstRuleEnrollmentEmployee</t>
   </si>
   <si>
@@ -375,6 +339,45 @@
   </si>
   <si>
     <t>"Over max employees per shift " + $SD</t>
+  </si>
+  <si>
+    <t>condition:assignedEmployees</t>
+  </si>
+  <si>
+    <t>condition:assignable</t>
+  </si>
+  <si>
+    <t>action:setAssignable</t>
+  </si>
+  <si>
+    <t>action:setDeletable</t>
+  </si>
+  <si>
+    <t>sub:autoAssignmentContext</t>
+  </si>
+  <si>
+    <t>sub:currentShift</t>
+  </si>
+  <si>
+    <t>condition:assignedShiftInDay</t>
+  </si>
+  <si>
+    <t>condition:isAssignable</t>
+  </si>
+  <si>
+    <t>condition:isEligible</t>
+  </si>
+  <si>
+    <t>condition:isEnrolled</t>
+  </si>
+  <si>
+    <t>condition:isAssigned</t>
+  </si>
+  <si>
+    <t>action:setEligible</t>
+  </si>
+  <si>
+    <t>condition:assignedShiftInWeek</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -467,6 +470,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -812,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300E403C-BA1A-49A4-A31C-A695E7440B6E}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,11 +829,12 @@
     <col min="3" max="3" width="41.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
     <col min="5" max="5" width="28" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
@@ -835,43 +842,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="F1" s="8"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="J1" s="8"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="J2" s="9"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="b">
         <v>1</v>
@@ -879,7 +886,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1">
         <v>100</v>
@@ -887,54 +894,54 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="G7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="8"/>
+      <c r="C8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -943,22 +950,22 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>54</v>
+      <c r="F9" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -966,151 +973,151 @@
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>34</v>
+        <v>110</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>103</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D11" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>55</v>
+        <v>77</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>60</v>
+        <v>94</v>
+      </c>
+      <c r="F12" t="s">
+        <v>52</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>60</v>
+      <c r="F13" t="s">
+        <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>5</v>
+      <c r="F16" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="8"/>
+      <c r="C17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="11"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -1118,148 +1125,148 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>9</v>
+        <v>101</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>104</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="D21" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>90</v>
+        <v>52</v>
+      </c>
+      <c r="F21" t="s">
+        <v>79</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="5"/>
       <c r="L23" s="7"/>
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="K24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1267,14 +1274,14 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
+      <c r="E25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1283,19 +1290,19 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>48</v>
+        <v>78</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H26" s="3">
         <v>1</v>
@@ -1303,14 +1310,14 @@
       <c r="I26" s="3">
         <v>1</v>
       </c>
-      <c r="J26" s="2" t="s">
-        <v>45</v>
+      <c r="J26" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="M26" s="2"/>
     </row>
@@ -1318,253 +1325,253 @@
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>7</v>
+        <v>107</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>113</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J27" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M27" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M27" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="F28" t="s">
+        <v>42</v>
       </c>
       <c r="G28" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
+      </c>
+      <c r="J28" t="s">
+        <v>38</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="F29" t="s">
+        <v>42</v>
       </c>
       <c r="G29" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>47</v>
+        <v>73</v>
+      </c>
+      <c r="J29" t="s">
+        <v>39</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="F30" t="s">
+        <v>42</v>
       </c>
       <c r="G30" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>47</v>
+        <v>89</v>
+      </c>
+      <c r="J30" t="s">
+        <v>39</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G31" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>47</v>
+      <c r="J31" t="s">
+        <v>39</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>57</v>
+        <v>84</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
       </c>
       <c r="G32" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>47</v>
+      <c r="J32" t="s">
+        <v>39</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="F34" s="8"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
+      <c r="J34" s="8"/>
       <c r="K34" s="7"/>
       <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>5</v>
+      <c r="J35" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
@@ -1572,14 +1579,14 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="8"/>
-      <c r="G36" s="8"/>
+      <c r="E36" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="J36" s="9"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
@@ -1587,31 +1594,31 @@
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H37" s="3">
         <v>1</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="L37" s="2"/>
     </row>
@@ -1619,280 +1626,280 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>7</v>
+        <v>107</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>113</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="I38" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L38" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L38" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="F39" t="s">
+        <v>42</v>
       </c>
       <c r="G39" s="1" t="b">
         <v>0</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
+      </c>
+      <c r="F40" t="s">
+        <v>42</v>
       </c>
       <c r="G40" s="1" t="b">
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G41" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>57</v>
+        <v>74</v>
+      </c>
+      <c r="F42" t="s">
+        <v>49</v>
       </c>
       <c r="G42" s="1" t="b">
         <v>1</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J42" s="1" t="s">
-        <v>90</v>
+        <v>39</v>
+      </c>
+      <c r="J42" t="s">
+        <v>79</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="F44" s="8"/>
       <c r="G44" s="5"/>
       <c r="H44" s="7"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
+      <c r="J44" s="8"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="H45" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>100</v>
+        <v>32</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
+      <c r="J46" s="9"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
+      <c r="J47" s="9"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>110</v>
+        <v>97</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>98</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>100</v>
+        <v>33</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
@@ -1901,30 +1908,30 @@
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
+      </c>
+      <c r="F49" t="s">
+        <v>66</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J49" s="1" t="b">
+        <v>58</v>
+      </c>
+      <c r="J49" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
@@ -1933,21 +1940,21 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
+      </c>
+      <c r="F50" t="s">
+        <v>68</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J50" s="1" t="b">
+        <v>58</v>
+      </c>
+      <c r="J50" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1974,6 +1981,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>

<commit_message>
feat: Add MQTT microservice, install mqtt package, add arduino mqtt-client code, add mosquitto-mqtt service to docker-compose file + config file, add test service + controller for mqtt microservice
</commit_message>
<xml_diff>
--- a/droolsServer/src/main/resources/dtables/drools_decisiontable.drl.xlsx
+++ b/droolsServer/src/main/resources/dtables/drools_decisiontable.drl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Ex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Smashminton\droolsServer\src\main\resources\dtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7574F11B-262B-48D1-B242-6948CE1B7BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BD3ADC-00C4-409F-9A98-E02010E6E17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BFDAF6E-2941-4913-A8C6-9531DFE6061F}"/>
   </bookViews>
@@ -221,9 +221,6 @@
     <t>"Set Eligible For: " + $E + " on " + $CSD</t>
   </si>
   <si>
-    <t>not(ShiftAssignment(getEmployee().equals($E), getShift().equals( $CSD)))</t>
-  </si>
-  <si>
     <t>modify($EE){ $1 }</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>"Already Assigned: " + $E + " on " + $CSD</t>
   </si>
   <si>
-    <t>ShiftAssignment(getEmployee().equals($E), getShift().equals( $CSD))</t>
-  </si>
-  <si>
     <t>FourthRuleEmployee</t>
   </si>
   <si>
@@ -378,6 +372,12 @@
   </si>
   <si>
     <t>condition:assignedShiftInWeek</t>
+  </si>
+  <si>
+    <t>ShiftAssignment(getEmployee().equals($E), getShift().equals($CSD))</t>
+  </si>
+  <si>
+    <t>not(ShiftAssignment(getEmployee().equals($E), getShift().equals($CSD)))</t>
   </si>
 </sst>
 </file>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300E403C-BA1A-49A4-A31C-A695E7440B6E}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -894,7 +894,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -973,19 +973,19 @@
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>104</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>11</v>
@@ -999,7 +999,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>41</v>
@@ -1008,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F11" t="s">
         <v>47</v>
@@ -1017,7 +1017,7 @@
         <v>59</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1025,7 +1025,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>41</v>
@@ -1034,16 +1034,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F12" t="s">
         <v>52</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>48</v>
@@ -1063,13 +1063,13 @@
         <v>52</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>53</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1145,16 +1145,16 @@
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>103</v>
-      </c>
       <c r="F19" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>11</v>
@@ -1203,10 +1203,10 @@
         <v>52</v>
       </c>
       <c r="F21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>34</v>
@@ -1214,7 +1214,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1296,7 +1296,7 @@
         <v>55</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>40</v>
@@ -1325,31 +1325,31 @@
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="F27" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G27" s="6" t="s">
+      <c r="H27" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="J27" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="I27" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="J27" s="10" t="s">
-        <v>112</v>
-      </c>
       <c r="K27" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>11</v>
@@ -1363,7 +1363,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>25</v>
@@ -1381,10 +1381,10 @@
         <v>0</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="J28" t="s">
         <v>38</v>
@@ -1393,7 +1393,7 @@
         <v>60</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1401,7 +1401,7 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>25</v>
@@ -1419,16 +1419,16 @@
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="J29" t="s">
         <v>39</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -1436,7 +1436,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>25</v>
@@ -1454,16 +1454,16 @@
         <v>1</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J30" t="s">
         <v>39</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1471,7 +1471,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>25</v>
@@ -1492,7 +1492,7 @@
         <v>44</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1500,7 +1500,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s">
         <v>49</v>
@@ -1512,13 +1512,13 @@
         <v>39</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1626,28 +1626,28 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="6" t="s">
+      <c r="F38" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="G38" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>111</v>
-      </c>
       <c r="I38" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>11</v>
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>38</v>
@@ -1714,13 +1714,13 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>35</v>
@@ -1760,7 +1760,7 @@
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F42" t="s">
         <v>49</v>
@@ -1772,7 +1772,7 @@
         <v>39</v>
       </c>
       <c r="J42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>45</v>
@@ -1823,7 +1823,7 @@
         <v>32</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -1852,13 +1852,13 @@
         <v>19</v>
       </c>
       <c r="E47" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F47" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>36</v>
@@ -1876,13 +1876,13 @@
         <v>16</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>11</v>
@@ -1891,7 +1891,7 @@
         <v>33</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1908,16 +1908,16 @@
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F49" t="s">
         <v>65</v>
       </c>
-      <c r="F49" t="s">
-        <v>66</v>
-      </c>
       <c r="G49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>58</v>
@@ -1940,16 +1940,16 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" t="s">
         <v>67</v>
       </c>
-      <c r="F50" t="s">
-        <v>68</v>
-      </c>
       <c r="G50" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
feat: implement fileWatcher for Excel changes instead of simply reload for it to work in prod mode, change Excel value data and align with client, update new package version, fix _homepage button gap responsive
</commit_message>
<xml_diff>
--- a/droolsServer/src/main/resources/dtables/drools_decisiontable.drl.xlsx
+++ b/droolsServer/src/main/resources/dtables/drools_decisiontable.drl.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\panthera\workspace\Smashminton\droolsServer\src\main\resources\dtables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Smashminton\droolsServer\src\main\resources\dtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D984327F-5DF1-4581-A0BE-916919ED768A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD32B634-13D6-4539-B12D-8C6A112FC944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{8BFDAF6E-2941-4913-A8C6-9531DFE6061F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8BFDAF6E-2941-4913-A8C6-9531DFE6061F}"/>
   </bookViews>
   <sheets>
     <sheet name="DroolsRules" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="105">
   <si>
     <t>RuleSet</t>
   </si>
@@ -170,12 +170,6 @@
     <t>ThirdRuleEmployee</t>
   </si>
   <si>
-    <t>"Over max shifts per day"</t>
-  </si>
-  <si>
-    <t>"Over max shifts per week"</t>
-  </si>
-  <si>
     <t>modify($SD) { $1 }</t>
   </si>
   <si>
@@ -197,9 +191,6 @@
     <t>setAssignable(false);</t>
   </si>
   <si>
-    <t>"Over max employees per shift"</t>
-  </si>
-  <si>
     <t>$C: AutoAssignmentContext()</t>
   </si>
   <si>
@@ -215,12 +206,6 @@
     <t>EmployeeSortingRule</t>
   </si>
   <si>
-    <t>"Set Assigble For: " + $SD</t>
-  </si>
-  <si>
-    <t>"Set Eligible For: " + $E + " on " + $CSD</t>
-  </si>
-  <si>
     <t>modify($EE){ $1 }</t>
   </si>
   <si>
@@ -251,9 +236,6 @@
     <t>sortEmployees($s)</t>
   </si>
   <si>
-    <t>"Already Assigned: " + $E + " on " + $CSD</t>
-  </si>
-  <si>
     <t>FourthRuleEmployee</t>
   </si>
   <si>
@@ -263,9 +245,6 @@
     <t>SecondRuleEnrollmentShift</t>
   </si>
   <si>
-    <t>ShiftEnrollment(getShift().equals($SD))</t>
-  </si>
-  <si>
     <t>getAssignedShiftInDay($CSD.getShiftDate())  $1</t>
   </si>
   <si>
@@ -293,18 +272,9 @@
     <t>EnrollmentEmployeeRule</t>
   </si>
   <si>
-    <t>ShiftEnrollment(getEmployee().equals($E), getShift().equals($CSD))</t>
-  </si>
-  <si>
     <t>NO-LOOP</t>
   </si>
   <si>
-    <t>not(ShiftEnrollment(getEmployee().equals($E), getShift().equals($CSD)))</t>
-  </si>
-  <si>
-    <t>"" + $E + " didn't enroll in " + $CSD</t>
-  </si>
-  <si>
     <t>RuleTable AssignableEnrollmentShifts</t>
   </si>
   <si>
@@ -314,12 +284,6 @@
     <t>ThirdRuleEnrollmentShift</t>
   </si>
   <si>
-    <t>not(ShiftEnrollment(getShift().equals($SD)))</t>
-  </si>
-  <si>
-    <t>"" + $SD + " didn't get enrolled"</t>
-  </si>
-  <si>
     <t>"Rule Sort Employee 2 Fired"</t>
   </si>
   <si>
@@ -332,9 +296,6 @@
     <t>com.example.model.Employee, com.example.model.Shift_Date, com.example.util.Sort, com.example.util.Sort.SortType, com.example.util.Sort.SortBy, com.example.model.EligibleEmployees, com.example.model.AssignableShifts, com.example.model.ShiftAssignments, com.example.model.ShiftAssignment, com.example.model.AutoAssignmentContext, com.example.model.ShiftEnrollment</t>
   </si>
   <si>
-    <t>"Over max employees per shift " + $SD</t>
-  </si>
-  <si>
     <t>condition:assignedEmployees</t>
   </si>
   <si>
@@ -371,13 +332,25 @@
     <t>condition:assignedShiftInWeek</t>
   </si>
   <si>
-    <t>ShiftAssignment(getEmployee().equals($E), getShift().equals($CSD))</t>
-  </si>
-  <si>
-    <t>not(ShiftAssignment(getEmployee().equals($E), getShift().equals($CSD)))</t>
-  </si>
-  <si>
     <t>setDeletable(false);</t>
+  </si>
+  <si>
+    <t>ShiftEnrollment(shift == $SD)</t>
+  </si>
+  <si>
+    <t>not(ShiftEnrollment(shift == $SD))</t>
+  </si>
+  <si>
+    <t>ShiftEnrollment(employee == $E, shift == $CSD)</t>
+  </si>
+  <si>
+    <t>not(ShiftEnrollment(employee == $E, shift == $CSD))</t>
+  </si>
+  <si>
+    <t>not(ShiftAssignment(employee == $E, shift == $CSD))</t>
+  </si>
+  <si>
+    <t>ShiftAssignment(employee == $E, shift == $CSD)</t>
   </si>
 </sst>
 </file>
@@ -818,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{300E403C-BA1A-49A4-A31C-A695E7440B6E}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +836,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -894,7 +867,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -950,7 +923,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>27</v>
@@ -959,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>36</v>
@@ -973,19 +946,19 @@
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>11</v>
@@ -999,7 +972,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>41</v>
@@ -1008,16 +981,13 @@
         <v>0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1025,7 +995,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>41</v>
@@ -1034,16 +1004,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1051,25 +1018,22 @@
         <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1125,16 +1089,16 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>36</v>
@@ -1145,16 +1109,16 @@
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>11</v>
@@ -1177,10 +1141,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>34</v>
@@ -1191,22 +1152,19 @@
         <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="F21" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>34</v>
@@ -1214,7 +1172,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1290,13 +1248,13 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>40</v>
@@ -1325,31 +1283,31 @@
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="J27" s="10" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>11</v>
@@ -1358,12 +1316,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>25</v>
@@ -1381,30 +1339,27 @@
         <v>0</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="J28" t="s">
         <v>38</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L28" s="1" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>25</v>
@@ -1422,24 +1377,21 @@
         <v>1</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J29" t="s">
         <v>39</v>
       </c>
-      <c r="L29" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="M29" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>25</v>
@@ -1457,16 +1409,14 @@
         <v>1</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="J30" t="s">
         <v>39</v>
       </c>
-      <c r="L30" s="4" t="s">
-        <v>88</v>
-      </c>
+      <c r="L30" s="4"/>
       <c r="M30" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1474,7 +1424,7 @@
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>25</v>
@@ -1483,7 +1433,7 @@
         <v>25</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G31" s="1" t="b">
         <v>1</v>
@@ -1491,11 +1441,8 @@
       <c r="J31" t="s">
         <v>39</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="M31" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1503,10 +1450,10 @@
         <v>6</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F32" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G32" s="1" t="b">
         <v>1</v>
@@ -1515,13 +1462,10 @@
         <v>39</v>
       </c>
       <c r="K32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
@@ -1597,13 +1541,13 @@
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>40</v>
@@ -1629,28 +1573,28 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>11</v>
@@ -1659,7 +1603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
@@ -1682,24 +1626,21 @@
         <v>0</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="L39" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>25</v>
@@ -1717,19 +1658,16 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="L40" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
@@ -1743,7 +1681,7 @@
         <v>25</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G41" s="1" t="b">
         <v>1</v>
@@ -1751,22 +1689,19 @@
       <c r="I41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="L41" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G42" s="1" t="b">
         <v>1</v>
@@ -1775,10 +1710,7 @@
         <v>39</v>
       </c>
       <c r="J42" t="s">
-        <v>77</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>35</v>
@@ -1826,7 +1758,7 @@
         <v>32</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -1855,13 +1787,13 @@
         <v>19</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H47" s="2" t="s">
         <v>36</v>
@@ -1879,13 +1811,13 @@
         <v>16</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>11</v>
@@ -1894,7 +1826,7 @@
         <v>33</v>
       </c>
       <c r="J48" s="10" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1911,19 +1843,19 @@
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F49" t="s">
+        <v>60</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="H49" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J49" t="b">
         <v>1</v>
@@ -1943,19 +1875,19 @@
         <v>1</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F50" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J50" t="b">
         <v>1</v>

</xml_diff>